<commit_message>
grafikler düzenlendi gid ve fotoğraf konuldu
yorumlar eklenilecek
</commit_message>
<xml_diff>
--- a/veri/Dunya_ve_Turkiye_bosanma_kaba_hizi.xlsx
+++ b/veri/Dunya_ve_Turkiye_bosanma_kaba_hizi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zahide\Desktop\is_analitik_odev\veri\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Excalibur\OneDrive\Belgeler\GitHub\muy665-bahar2025-takim-R_amam_soRmam_biR_daha\veri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26FF70D2-A3CF-4C8F-96A2-FF4A9B9AD55D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74944499-AAB7-423A-8DC8-E95BBBA35D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Türkiye</t>
   </si>
@@ -45,9 +45,6 @@
     <t>ABD</t>
   </si>
   <si>
-    <t>Hindistan</t>
-  </si>
-  <si>
     <t>Japonya</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
     <t>2,4</t>
   </si>
   <si>
-    <t>0,01</t>
-  </si>
-  <si>
     <t>1,5</t>
   </si>
   <si>
@@ -99,7 +93,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -172,7 +166,9 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{21077257-463C-4D71-A452-F54718EC284C}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -447,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,13 +458,13 @@
   <sheetData>
     <row r="1" spans="1:9" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D1" s="6"/>
     </row>
@@ -480,7 +476,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" s="7"/>
     </row>
@@ -492,7 +488,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" s="7"/>
     </row>
@@ -504,7 +500,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="7"/>
     </row>
@@ -516,7 +512,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" s="7"/>
     </row>
@@ -528,7 +524,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" s="7"/>
     </row>
@@ -540,7 +536,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="7"/>
     </row>
@@ -552,7 +548,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="7"/>
     </row>
@@ -564,7 +560,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" s="7"/>
     </row>
@@ -576,20 +572,14 @@
         <v>8</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" s="7"/>
     </row>
     <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="9">
-        <v>2022</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>22</v>
-      </c>
+      <c r="A11" s="5"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
       <c r="D11" s="7"/>
     </row>
     <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -603,19 +593,16 @@
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
       <c r="D13" s="7"/>
+      <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="7"/>
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="5"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="7"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C16" s="2"/>
@@ -637,9 +624,6 @@
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C22" s="2"/>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C23" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -648,12 +632,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6c027cd6-060d-4002-8ef0-4718453e0c3b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="47a50c3d-6af1-47c6-b42b-2f6d34f88ebf" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -846,20 +832,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6c027cd6-060d-4002-8ef0-4718453e0c3b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="47a50c3d-6af1-47c6-b42b-2f6d34f88ebf" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B4C3D81-22C5-4858-A868-B528ACD7E680}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7E01AE8-7CB9-4574-BC93-202771FC1EB6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6c027cd6-060d-4002-8ef0-4718453e0c3b"/>
+    <ds:schemaRef ds:uri="47a50c3d-6af1-47c6-b42b-2f6d34f88ebf"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -884,12 +871,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7E01AE8-7CB9-4574-BC93-202771FC1EB6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B4C3D81-22C5-4858-A868-B528ACD7E680}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="6c027cd6-060d-4002-8ef0-4718453e0c3b"/>
-    <ds:schemaRef ds:uri="47a50c3d-6af1-47c6-b42b-2f6d34f88ebf"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>